<commit_message>
update about page with description and main for long_legs
</commit_message>
<xml_diff>
--- a/csv_database/xlsx/filter.xlsx
+++ b/csv_database/xlsx/filter.xlsx
@@ -1039,8 +1039,8 @@
   <dimension ref="A1:AB120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D79" sqref="D79"/>
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J65" sqref="J65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>